<commit_message>
macOS 的 GUI crash 問題
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,7 +535,75 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-07-07 15:48:43</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-07-07 15:49:02</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-07-07 15:49:44</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-07-07 15:50:06</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>xuan_3</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>